<commit_message>
fixed a bug in the run estimation formula
</commit_message>
<xml_diff>
--- a/Metricas_CNV.xlsx
+++ b/Metricas_CNV.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="16">
   <si>
     <t>Maze</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>BFS</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>Velocity affects every strategy in the same way, so a lower velocity means a higher cost request</t>
   </si>
   <si>
     <t xml:space="preserve">Conclusão: </t>
@@ -439,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -460,35 +454,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -516,9 +510,10 @@
       <c r="H2" s="1">
         <v>5063</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>3346294917</v>
       </c>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
@@ -545,6 +540,10 @@
       <c r="H3" s="1">
         <v>5063</v>
       </c>
+      <c r="I3" s="1">
+        <v>2777425413</v>
+      </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
@@ -571,6 +570,10 @@
       <c r="H4" s="1">
         <v>5063</v>
       </c>
+      <c r="I4" s="1">
+        <v>2375870469</v>
+      </c>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
@@ -597,6 +600,10 @@
       <c r="H5" s="1">
         <v>5063</v>
       </c>
+      <c r="I5" s="1">
+        <v>2091435717</v>
+      </c>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
@@ -623,6 +630,10 @@
       <c r="H6" s="1">
         <v>5063</v>
       </c>
+      <c r="I6" s="1">
+        <v>1857195333</v>
+      </c>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
@@ -649,6 +660,10 @@
       <c r="H7" s="1">
         <v>5063</v>
       </c>
+      <c r="I7" s="1">
+        <v>1673149317</v>
+      </c>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
@@ -659,6 +674,8 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
@@ -685,9 +702,10 @@
       <c r="H9" s="1">
         <v>6</v>
       </c>
-      <c r="I9">
-        <v>2136335173</v>
-      </c>
+      <c r="I9" s="1">
+        <v>2139035976</v>
+      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
@@ -714,6 +732,10 @@
       <c r="H10" s="1">
         <v>6</v>
       </c>
+      <c r="I10" s="1">
+        <v>1775400264</v>
+      </c>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
@@ -740,9 +762,10 @@
       <c r="H11" s="1">
         <v>6</v>
       </c>
-      <c r="I11">
-        <v>1516798661</v>
-      </c>
+      <c r="I11" s="1">
+        <v>1518716232</v>
+      </c>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
@@ -769,6 +792,10 @@
       <c r="H12" s="1">
         <v>6</v>
       </c>
+      <c r="I12" s="1">
+        <v>1336898376</v>
+      </c>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
@@ -795,6 +822,10 @@
       <c r="H13" s="1">
         <v>6</v>
       </c>
+      <c r="I13" s="1">
+        <v>1187166024</v>
+      </c>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
@@ -821,9 +852,10 @@
       <c r="H14" s="1">
         <v>6</v>
       </c>
-      <c r="I14">
-        <v>1068168773</v>
-      </c>
+      <c r="I14" s="1">
+        <v>1069519176</v>
+      </c>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
@@ -834,6 +866,8 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
@@ -860,9 +894,10 @@
       <c r="H16" s="1">
         <v>8</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>8431906966</v>
       </c>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
@@ -889,9 +924,10 @@
       <c r="H17" s="1">
         <v>8</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>6998484374</v>
       </c>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
@@ -918,9 +954,10 @@
       <c r="H18" s="1">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>5986656662</v>
       </c>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
@@ -947,6 +984,10 @@
       <c r="H19" s="1">
         <v>8</v>
       </c>
+      <c r="I19" s="1">
+        <v>5269945366</v>
+      </c>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
@@ -973,6 +1014,10 @@
       <c r="H20" s="1">
         <v>8</v>
       </c>
+      <c r="I20" s="1">
+        <v>4679712534</v>
+      </c>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
@@ -999,6 +1044,10 @@
       <c r="H21" s="1">
         <v>8</v>
       </c>
+      <c r="I21" s="1">
+        <v>4215958166</v>
+      </c>
+      <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
@@ -1009,6 +1058,8 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
@@ -1035,7 +1086,8 @@
       <c r="H23" s="1">
         <v>5063</v>
       </c>
-      <c r="J23">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
         <v>4006778520</v>
       </c>
     </row>
@@ -1064,6 +1116,10 @@
       <c r="H24" s="1">
         <v>5063</v>
       </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1">
+        <v>4006778520</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
@@ -1090,6 +1146,10 @@
       <c r="H25" s="1">
         <v>5063</v>
       </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <v>4006778520</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
@@ -1116,6 +1176,10 @@
       <c r="H26" s="1">
         <v>5063</v>
       </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1">
+        <v>4006778520</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
@@ -1142,6 +1206,10 @@
       <c r="H27" s="1">
         <v>5063</v>
       </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1">
+        <v>4006778520</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
@@ -1167,6 +1235,10 @@
       </c>
       <c r="H28" s="1">
         <v>5063</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
+        <v>4006778520</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
@@ -1178,6 +1250,8 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
@@ -1204,7 +1278,8 @@
       <c r="H30" s="1">
         <v>6</v>
       </c>
-      <c r="J30">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1">
         <v>314727159</v>
       </c>
     </row>
@@ -1233,6 +1308,10 @@
       <c r="H31" s="1">
         <v>6</v>
       </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1">
+        <v>314727159</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
@@ -1259,6 +1338,10 @@
       <c r="H32" s="1">
         <v>6</v>
       </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1">
+        <v>314727159</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
@@ -1285,6 +1368,10 @@
       <c r="H33" s="1">
         <v>6</v>
       </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1">
+        <v>314727159</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
@@ -1311,6 +1398,10 @@
       <c r="H34" s="1">
         <v>6</v>
       </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1">
+        <v>314727159</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
@@ -1337,7 +1428,8 @@
       <c r="H35" s="1">
         <v>6</v>
       </c>
-      <c r="J35">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1">
         <v>314727159</v>
       </c>
     </row>
@@ -1350,6 +1442,8 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
@@ -1376,7 +1470,8 @@
       <c r="H37" s="1">
         <v>8</v>
       </c>
-      <c r="J37">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1">
         <v>6054763095</v>
       </c>
     </row>
@@ -1405,6 +1500,10 @@
       <c r="H38" s="1">
         <v>8</v>
       </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1">
+        <v>6054763095</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
@@ -1431,6 +1530,10 @@
       <c r="H39" s="1">
         <v>8</v>
       </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1">
+        <v>6054763095</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
@@ -1457,6 +1560,10 @@
       <c r="H40" s="1">
         <v>8</v>
       </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1">
+        <v>6054763095</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
@@ -1483,6 +1590,10 @@
       <c r="H41" s="1">
         <v>8</v>
       </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1">
+        <v>6054763095</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
@@ -1509,15 +1620,9 @@
       <c r="H42" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>14</v>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1">
+        <v>6054763095</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1635,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2059,7 +2164,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>